<commit_message>
More outputs, one file
</commit_message>
<xml_diff>
--- a/outputs.xlsx
+++ b/outputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sasreena/p2clru/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{948389A2-2E61-B849-A343-AE16DB60B4EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{4EEDF0E6-3749-D248-9807-F06BE7495A21}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16700" xr2:uid="{AA3B79A8-98A5-EC49-8EEA-546486CF1BEC}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16660" xr2:uid="{AA3B79A8-98A5-EC49-8EEA-546486CF1BEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Frame size</t>
   </si>
@@ -45,15 +45,26 @@
     <t>LRU</t>
   </si>
   <si>
-    <t>Power of 2 choices in LRU</t>
+    <t>Power of 2 choices using LRU</t>
+  </si>
+  <si>
+    <t>Sl. No.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -81,13 +92,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,124 +415,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8ACC722-92A7-784F-98F5-2ADBCA9A8379}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>100</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>50</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>81</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.67300000000000004</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>81</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.48</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <v>10</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>75</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>45</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>63</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>0.59199999999999997</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>62</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.46600000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>75</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>40</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>68</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>0.377</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>69</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>0.318</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>45</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>34</v>
+      </c>
+      <c r="F7">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="G7">
+        <v>36</v>
+      </c>
+      <c r="H7">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>0.128</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>